<commit_message>
Ordner fuer Protokolle, Arbeitszeiten IF
</commit_message>
<xml_diff>
--- a/Dokumente/Arbeitszeiten/Ingmar_Fila.xlsx
+++ b/Dokumente/Arbeitszeiten/Ingmar_Fila.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Arbeitszeiten</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Informationen sammeln, experimentieren jQueryUI, Erstellung Prototyp in JQueryUI</t>
+  </si>
+  <si>
+    <t>Arbeiten an GUI</t>
   </si>
 </sst>
 </file>
@@ -475,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1193,12 @@
       <c r="A60" s="1">
         <v>41782</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>

</xml_diff>

<commit_message>
GUI 0.7b + Arbeitszeiten IF
</commit_message>
<xml_diff>
--- a/Dokumente/Arbeitszeiten/Ingmar_Fila.xlsx
+++ b/Dokumente/Arbeitszeiten/Ingmar_Fila.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Arbeitszeiten</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Urlaub</t>
+  </si>
+  <si>
+    <t>5h</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83:J83"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1543,12 @@
       <c r="A88" s="1">
         <v>41807</v>
       </c>
-      <c r="D88" s="2"/>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -1564,7 +1572,12 @@
       <c r="A90" s="1">
         <v>41809</v>
       </c>
-      <c r="D90" s="2"/>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -1600,7 +1613,12 @@
       <c r="A93" s="1">
         <v>41812</v>
       </c>
-      <c r="D93" s="2"/>
+      <c r="C93" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -1624,7 +1642,12 @@
       <c r="A95" s="1">
         <v>41814</v>
       </c>
-      <c r="D95" s="2"/>
+      <c r="C95" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -1636,7 +1659,12 @@
       <c r="A96" s="1">
         <v>41815</v>
       </c>
-      <c r="D96" s="2"/>
+      <c r="C96" t="s">
+        <v>17</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -1879,17 +1907,87 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D115:J115"/>
+    <mergeCell ref="D116:J116"/>
+    <mergeCell ref="D117:J117"/>
+    <mergeCell ref="D109:J109"/>
+    <mergeCell ref="D110:J110"/>
+    <mergeCell ref="D111:J111"/>
+    <mergeCell ref="D112:J112"/>
+    <mergeCell ref="D113:J113"/>
+    <mergeCell ref="D114:J114"/>
+    <mergeCell ref="D100:J100"/>
+    <mergeCell ref="D101:J101"/>
+    <mergeCell ref="D105:J105"/>
+    <mergeCell ref="D106:J106"/>
+    <mergeCell ref="D107:J107"/>
+    <mergeCell ref="D108:J108"/>
+    <mergeCell ref="D94:J94"/>
+    <mergeCell ref="D95:J95"/>
+    <mergeCell ref="D96:J96"/>
+    <mergeCell ref="D97:J97"/>
+    <mergeCell ref="D98:J98"/>
+    <mergeCell ref="D99:J99"/>
+    <mergeCell ref="D88:J88"/>
+    <mergeCell ref="D89:J89"/>
+    <mergeCell ref="D90:J90"/>
+    <mergeCell ref="D91:J91"/>
+    <mergeCell ref="D92:J92"/>
+    <mergeCell ref="D93:J93"/>
+    <mergeCell ref="D82:J82"/>
+    <mergeCell ref="D83:J83"/>
+    <mergeCell ref="D84:J84"/>
+    <mergeCell ref="D85:J85"/>
+    <mergeCell ref="D86:J86"/>
+    <mergeCell ref="D87:J87"/>
+    <mergeCell ref="D76:J76"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="D78:J78"/>
+    <mergeCell ref="D79:J79"/>
+    <mergeCell ref="D80:J80"/>
+    <mergeCell ref="D81:J81"/>
+    <mergeCell ref="D67:J67"/>
+    <mergeCell ref="D68:J68"/>
+    <mergeCell ref="D72:J72"/>
+    <mergeCell ref="D73:J73"/>
+    <mergeCell ref="D74:J74"/>
+    <mergeCell ref="D75:J75"/>
+    <mergeCell ref="D61:J61"/>
+    <mergeCell ref="D62:J62"/>
+    <mergeCell ref="D63:J63"/>
+    <mergeCell ref="D64:J64"/>
+    <mergeCell ref="D65:J65"/>
+    <mergeCell ref="D66:J66"/>
+    <mergeCell ref="D55:J55"/>
+    <mergeCell ref="D56:J56"/>
+    <mergeCell ref="D57:J57"/>
+    <mergeCell ref="D58:J58"/>
+    <mergeCell ref="D59:J59"/>
+    <mergeCell ref="D60:J60"/>
+    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="D53:J53"/>
+    <mergeCell ref="D54:J54"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="D41:J41"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="D30:J30"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="D33:J33"/>
     <mergeCell ref="D22:J22"/>
     <mergeCell ref="D23:J23"/>
     <mergeCell ref="D24:J24"/>
@@ -1902,87 +2000,17 @@
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="D41:J41"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="D30:J30"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="D49:J49"/>
-    <mergeCell ref="D50:J50"/>
-    <mergeCell ref="D51:J51"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="D53:J53"/>
-    <mergeCell ref="D54:J54"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="D48:J48"/>
-    <mergeCell ref="D61:J61"/>
-    <mergeCell ref="D62:J62"/>
-    <mergeCell ref="D63:J63"/>
-    <mergeCell ref="D64:J64"/>
-    <mergeCell ref="D65:J65"/>
-    <mergeCell ref="D66:J66"/>
-    <mergeCell ref="D55:J55"/>
-    <mergeCell ref="D56:J56"/>
-    <mergeCell ref="D57:J57"/>
-    <mergeCell ref="D58:J58"/>
-    <mergeCell ref="D59:J59"/>
-    <mergeCell ref="D60:J60"/>
-    <mergeCell ref="D76:J76"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="D78:J78"/>
-    <mergeCell ref="D79:J79"/>
-    <mergeCell ref="D80:J80"/>
-    <mergeCell ref="D81:J81"/>
-    <mergeCell ref="D67:J67"/>
-    <mergeCell ref="D68:J68"/>
-    <mergeCell ref="D72:J72"/>
-    <mergeCell ref="D73:J73"/>
-    <mergeCell ref="D74:J74"/>
-    <mergeCell ref="D75:J75"/>
-    <mergeCell ref="D88:J88"/>
-    <mergeCell ref="D89:J89"/>
-    <mergeCell ref="D90:J90"/>
-    <mergeCell ref="D91:J91"/>
-    <mergeCell ref="D92:J92"/>
-    <mergeCell ref="D93:J93"/>
-    <mergeCell ref="D82:J82"/>
-    <mergeCell ref="D83:J83"/>
-    <mergeCell ref="D84:J84"/>
-    <mergeCell ref="D85:J85"/>
-    <mergeCell ref="D86:J86"/>
-    <mergeCell ref="D87:J87"/>
-    <mergeCell ref="D100:J100"/>
-    <mergeCell ref="D101:J101"/>
-    <mergeCell ref="D105:J105"/>
-    <mergeCell ref="D106:J106"/>
-    <mergeCell ref="D107:J107"/>
-    <mergeCell ref="D108:J108"/>
-    <mergeCell ref="D94:J94"/>
-    <mergeCell ref="D95:J95"/>
-    <mergeCell ref="D96:J96"/>
-    <mergeCell ref="D97:J97"/>
-    <mergeCell ref="D98:J98"/>
-    <mergeCell ref="D99:J99"/>
-    <mergeCell ref="D115:J115"/>
-    <mergeCell ref="D116:J116"/>
-    <mergeCell ref="D117:J117"/>
-    <mergeCell ref="D109:J109"/>
-    <mergeCell ref="D110:J110"/>
-    <mergeCell ref="D111:J111"/>
-    <mergeCell ref="D112:J112"/>
-    <mergeCell ref="D113:J113"/>
-    <mergeCell ref="D114:J114"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GUI & Arbeitszeiten IF
</commit_message>
<xml_diff>
--- a/Dokumente/Arbeitszeiten/Ingmar_Fila.xlsx
+++ b/Dokumente/Arbeitszeiten/Ingmar_Fila.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Arbeitszeiten</t>
   </si>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,7 +1700,12 @@
       <c r="A99" s="1">
         <v>41818</v>
       </c>
-      <c r="D99" s="2"/>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -1759,7 +1764,12 @@
       <c r="A106" s="1">
         <v>41822</v>
       </c>
-      <c r="D106" s="2"/>
+      <c r="C106" t="s">
+        <v>17</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -1907,15 +1917,89 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="D115:J115"/>
-    <mergeCell ref="D116:J116"/>
-    <mergeCell ref="D117:J117"/>
-    <mergeCell ref="D109:J109"/>
-    <mergeCell ref="D110:J110"/>
-    <mergeCell ref="D111:J111"/>
-    <mergeCell ref="D112:J112"/>
-    <mergeCell ref="D113:J113"/>
-    <mergeCell ref="D114:J114"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="D41:J41"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="D30:J30"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="D53:J53"/>
+    <mergeCell ref="D54:J54"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="D61:J61"/>
+    <mergeCell ref="D62:J62"/>
+    <mergeCell ref="D63:J63"/>
+    <mergeCell ref="D64:J64"/>
+    <mergeCell ref="D65:J65"/>
+    <mergeCell ref="D66:J66"/>
+    <mergeCell ref="D55:J55"/>
+    <mergeCell ref="D56:J56"/>
+    <mergeCell ref="D57:J57"/>
+    <mergeCell ref="D58:J58"/>
+    <mergeCell ref="D59:J59"/>
+    <mergeCell ref="D60:J60"/>
+    <mergeCell ref="D76:J76"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="D78:J78"/>
+    <mergeCell ref="D79:J79"/>
+    <mergeCell ref="D80:J80"/>
+    <mergeCell ref="D81:J81"/>
+    <mergeCell ref="D67:J67"/>
+    <mergeCell ref="D68:J68"/>
+    <mergeCell ref="D72:J72"/>
+    <mergeCell ref="D73:J73"/>
+    <mergeCell ref="D74:J74"/>
+    <mergeCell ref="D75:J75"/>
+    <mergeCell ref="D88:J88"/>
+    <mergeCell ref="D89:J89"/>
+    <mergeCell ref="D90:J90"/>
+    <mergeCell ref="D91:J91"/>
+    <mergeCell ref="D92:J92"/>
+    <mergeCell ref="D93:J93"/>
+    <mergeCell ref="D82:J82"/>
+    <mergeCell ref="D83:J83"/>
+    <mergeCell ref="D84:J84"/>
+    <mergeCell ref="D85:J85"/>
+    <mergeCell ref="D86:J86"/>
+    <mergeCell ref="D87:J87"/>
     <mergeCell ref="D100:J100"/>
     <mergeCell ref="D101:J101"/>
     <mergeCell ref="D105:J105"/>
@@ -1928,89 +2012,15 @@
     <mergeCell ref="D97:J97"/>
     <mergeCell ref="D98:J98"/>
     <mergeCell ref="D99:J99"/>
-    <mergeCell ref="D88:J88"/>
-    <mergeCell ref="D89:J89"/>
-    <mergeCell ref="D90:J90"/>
-    <mergeCell ref="D91:J91"/>
-    <mergeCell ref="D92:J92"/>
-    <mergeCell ref="D93:J93"/>
-    <mergeCell ref="D82:J82"/>
-    <mergeCell ref="D83:J83"/>
-    <mergeCell ref="D84:J84"/>
-    <mergeCell ref="D85:J85"/>
-    <mergeCell ref="D86:J86"/>
-    <mergeCell ref="D87:J87"/>
-    <mergeCell ref="D76:J76"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="D78:J78"/>
-    <mergeCell ref="D79:J79"/>
-    <mergeCell ref="D80:J80"/>
-    <mergeCell ref="D81:J81"/>
-    <mergeCell ref="D67:J67"/>
-    <mergeCell ref="D68:J68"/>
-    <mergeCell ref="D72:J72"/>
-    <mergeCell ref="D73:J73"/>
-    <mergeCell ref="D74:J74"/>
-    <mergeCell ref="D75:J75"/>
-    <mergeCell ref="D61:J61"/>
-    <mergeCell ref="D62:J62"/>
-    <mergeCell ref="D63:J63"/>
-    <mergeCell ref="D64:J64"/>
-    <mergeCell ref="D65:J65"/>
-    <mergeCell ref="D66:J66"/>
-    <mergeCell ref="D55:J55"/>
-    <mergeCell ref="D56:J56"/>
-    <mergeCell ref="D57:J57"/>
-    <mergeCell ref="D58:J58"/>
-    <mergeCell ref="D59:J59"/>
-    <mergeCell ref="D60:J60"/>
-    <mergeCell ref="D49:J49"/>
-    <mergeCell ref="D50:J50"/>
-    <mergeCell ref="D51:J51"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="D53:J53"/>
-    <mergeCell ref="D54:J54"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="D48:J48"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="D41:J41"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="D30:J30"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D115:J115"/>
+    <mergeCell ref="D116:J116"/>
+    <mergeCell ref="D117:J117"/>
+    <mergeCell ref="D109:J109"/>
+    <mergeCell ref="D110:J110"/>
+    <mergeCell ref="D111:J111"/>
+    <mergeCell ref="D112:J112"/>
+    <mergeCell ref="D113:J113"/>
+    <mergeCell ref="D114:J114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>